<commit_message>
DAS Lab 5 Added
</commit_message>
<xml_diff>
--- a/das/DAS.xlsx
+++ b/das/DAS.xlsx
@@ -9,15 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9885" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="COREL" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
-    <sheet name="Descriptive_Stats" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="COREL2" sheetId="7" r:id="rId2"/>
+    <sheet name="COREL3" sheetId="8" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId6"/>
+    <sheet name="Descriptive_Stats" sheetId="3" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="n" localSheetId="2">COREL3!$L$12</definedName>
+    <definedName name="n">COREL2!$K$6</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -304,8 +310,417 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>4mca</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 1
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 3
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 6</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 7
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 9</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 10</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 11</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 12</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>4mca</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 1
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 3
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>4mca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Step 6</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>DESCRIPTIVE STATISTICS</t>
   </si>
@@ -575,6 +990,83 @@
   <si>
     <t>ERROR</t>
   </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Total Savings</t>
+  </si>
+  <si>
+    <t>Sl</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Co Variance</t>
+  </si>
+  <si>
+    <t>Co Relation</t>
+  </si>
+  <si>
+    <t>Slope (M)</t>
+  </si>
+  <si>
+    <t>Intercept ( C)</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Observed</t>
+  </si>
+  <si>
+    <t>COREL(X,Y)</t>
+  </si>
+  <si>
+    <r>
+      <t>y=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>213.690476</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10.892857</t>
+    </r>
+  </si>
+  <si>
+    <t>Slope(X,Y)</t>
+  </si>
+  <si>
+    <t>Intercept(X,Y)</t>
+  </si>
 </sst>
 </file>
 
@@ -582,9 +1074,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -724,6 +1216,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -757,7 +1272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -774,31 +1289,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -824,6 +1319,52 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -842,51 +1383,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1123,11 +1636,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="288257232"/>
-        <c:axId val="288257624"/>
+        <c:axId val="354225432"/>
+        <c:axId val="354225824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="288257232"/>
+        <c:axId val="354225432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1184,12 +1697,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288257624"/>
+        <c:crossAx val="354225824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="288257624"/>
+        <c:axId val="354225824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1246,7 +1759,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288257232"/>
+        <c:crossAx val="354225432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1558,9 +2071,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:val>
@@ -4525,8 +5036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4538,10 +5049,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="42"/>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -4552,34 +5063,34 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="37" t="s">
+      <c r="M3" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="37"/>
+      <c r="N3" s="31"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -4588,14 +5099,14 @@
       <c r="B4">
         <v>97</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="17">
         <v>12.5</v>
       </c>
       <c r="D4">
         <f>B4-$B$17</f>
         <v>42.5</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="17">
         <f>C4-$C$17</f>
         <v>4.25</v>
       </c>
@@ -4619,14 +5130,14 @@
       <c r="B5">
         <v>93</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="17">
         <v>12.5</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D15" si="0">B5-$B$17</f>
         <v>38.5</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="17">
         <f t="shared" ref="E5:E15" si="1">C5-$C$17</f>
         <v>4.25</v>
       </c>
@@ -4650,14 +5161,14 @@
       <c r="B6">
         <v>88</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="17">
         <v>8</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
         <v>33.5</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="17">
         <f t="shared" si="1"/>
         <v>-0.25</v>
       </c>
@@ -4673,10 +5184,10 @@
         <f t="shared" si="4"/>
         <v>-8.375</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="33">
+      <c r="K6" s="24">
         <v>12</v>
       </c>
     </row>
@@ -4687,14 +5198,14 @@
       <c r="B7">
         <v>81</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="17">
         <v>9.5</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
         <v>26.5</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="17">
         <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
@@ -4718,14 +5229,14 @@
       <c r="B8">
         <v>75</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="17">
         <v>16.5</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
         <v>20.5</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="17">
         <f t="shared" si="1"/>
         <v>8.25</v>
       </c>
@@ -4749,14 +5260,14 @@
       <c r="B9">
         <v>57</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="17">
         <v>11</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="17">
         <f t="shared" si="1"/>
         <v>2.75</v>
       </c>
@@ -4780,14 +5291,14 @@
       <c r="B10">
         <v>52</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="17">
         <v>10.5</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
         <v>-2.5</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="17">
         <f t="shared" si="1"/>
         <v>2.25</v>
       </c>
@@ -4811,14 +5322,14 @@
       <c r="B11">
         <v>45</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="17">
         <v>9</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
         <v>-9.5</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="17">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
@@ -4842,14 +5353,14 @@
       <c r="B12">
         <v>28</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="17">
         <v>6</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
         <v>-26.5</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="17">
         <f t="shared" si="1"/>
         <v>-2.25</v>
       </c>
@@ -4873,14 +5384,14 @@
       <c r="B13">
         <v>15</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="17">
         <v>1.5</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
         <v>-39.5</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="17">
         <f t="shared" si="1"/>
         <v>-6.75</v>
       </c>
@@ -4904,14 +5415,14 @@
       <c r="B14">
         <v>12</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="17">
         <v>1</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
         <v>-42.5</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="17">
         <f t="shared" si="1"/>
         <v>-7.25</v>
       </c>
@@ -4935,14 +5446,14 @@
       <c r="B15">
         <v>11</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="17">
         <v>1</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
         <v>-43.5</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="17">
         <f t="shared" si="1"/>
         <v>-7.25</v>
       </c>
@@ -4960,269 +5471,269 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="24" t="str">
+      <c r="D16" s="18" t="str">
         <f>D3</f>
         <v>X-X'</v>
       </c>
-      <c r="E16" s="24" t="str">
+      <c r="E16" s="18" t="str">
         <f>E3</f>
         <v>Y-Y'</v>
       </c>
-      <c r="F16" s="24" t="str">
+      <c r="F16" s="18" t="str">
         <f>F3</f>
         <v>(X-X')2</v>
       </c>
-      <c r="G16" s="24" t="str">
+      <c r="G16" s="18" t="str">
         <f>G3</f>
         <v>(Y-Y')2</v>
       </c>
-      <c r="H16" s="24" t="str">
+      <c r="H16" s="18" t="str">
         <f>H3</f>
         <v>(X-X')*(Y-Y')</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="15">
         <f>AVERAGE(B4:B15)</f>
         <v>54.5</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="15">
         <f>AVERAGE(C4:C15)</f>
         <v>8.25</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="15">
         <f t="shared" ref="D17:H17" si="5">AVERAGE(D4:D15)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="15">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="15">
         <f t="shared" si="5"/>
         <v>966.41666666666663</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="15">
         <f t="shared" si="5"/>
         <v>22.895833333333332</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="15">
         <f t="shared" si="5"/>
         <v>123.5</v>
       </c>
-      <c r="M17" s="22" t="s">
+      <c r="M17" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="N17" s="22"/>
+      <c r="N17" s="32"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15">
         <f>SUM(F4:F15)</f>
         <v>11597</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="15">
         <f t="shared" ref="G19:H19" si="6">SUM(G4:G15)</f>
         <v>274.75</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="15">
         <f t="shared" si="6"/>
         <v>1482</v>
       </c>
-      <c r="M19" s="22" t="s">
+      <c r="M19" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="N19" s="22"/>
+      <c r="N19" s="32"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15">
         <f>F19/($K$6-1)</f>
         <v>1054.2727272727273</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="15">
         <f>G19/($K$6-1)</f>
         <v>24.977272727272727</v>
       </c>
-      <c r="H21" s="21"/>
-      <c r="M21" s="22" t="s">
+      <c r="H21" s="15"/>
+      <c r="M21" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="N21" s="22"/>
+      <c r="N21" s="32"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15">
         <f>SQRT(F21)</f>
         <v>32.469566170072667</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="15">
         <f t="shared" ref="G23" si="7">SQRT(G21)</f>
         <v>4.997726755963428</v>
       </c>
-      <c r="H23" s="21"/>
-      <c r="M23" s="22" t="s">
+      <c r="H23" s="15"/>
+      <c r="M23" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="N23" s="22"/>
+      <c r="N23" s="32"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15">
         <f>H19/(K6-1)</f>
         <v>134.72727272727272</v>
       </c>
-      <c r="M25" s="22" t="s">
+      <c r="M25" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="N25" s="22"/>
+      <c r="N25" s="32"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J26" s="36" t="s">
+      <c r="J26" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22">
         <f>H25/(F23*G23)</f>
         <v>0.83024548881658089</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J27" s="35">
+      <c r="J27" s="36">
         <f>CORREL(B4:B15,C4:C15)</f>
         <v>0.83024548881658111</v>
       </c>
-      <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="22" t="s">
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="N27" s="22"/>
+      <c r="N27" s="32"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="39">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="26">
         <f>(H27*G23)/F23</f>
         <v>0.12779167025954985</v>
       </c>
-      <c r="M29" s="22" t="s">
+      <c r="M29" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="N29" s="22"/>
+      <c r="N29" s="32"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="40">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="27">
         <f>C17-(H29*B17)</f>
         <v>1.2853539708545334</v>
       </c>
-      <c r="M31" s="22" t="s">
+      <c r="M31" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="N31" s="22"/>
+      <c r="N31" s="32"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I33" s="38" t="s">
+      <c r="I33" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="38"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I34" s="38"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="38"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="33"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="37"/>
+      <c r="C36" s="31"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="5" t="s">
@@ -5237,7 +5748,7 @@
         <f>($H$29*B39)+$H$31</f>
         <v>13.681145986030868</v>
       </c>
-      <c r="D39" s="43">
+      <c r="D39" s="30">
         <f>C4-C39</f>
         <v>-1.1811459860308684</v>
       </c>
@@ -5250,7 +5761,7 @@
         <f t="shared" ref="C40:C41" si="8">($H$29*B40)+$H$31</f>
         <v>13.169979304992669</v>
       </c>
-      <c r="D40" s="43">
+      <c r="D40" s="30">
         <f t="shared" ref="D40:D41" si="9">C5-C40</f>
         <v>-0.669979304992669</v>
       </c>
@@ -5263,18 +5774,13 @@
         <f t="shared" si="8"/>
         <v>12.53102095369492</v>
       </c>
-      <c r="D41" s="43">
+      <c r="D41" s="30">
         <f t="shared" si="9"/>
         <v>-4.5310209536949202</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="I33:M34"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="J26:L26"/>
     <mergeCell ref="J27:L27"/>
@@ -5284,6 +5790,11 @@
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="M17:N17"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="I33:M34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5292,6 +5803,1328 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="31"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="17">
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <f>B4-$B$13</f>
+        <v>-3.5</v>
+      </c>
+      <c r="E4" s="17">
+        <f>C4-$C$13</f>
+        <v>-772.5</v>
+      </c>
+      <c r="F4">
+        <f>POWER(D4,2)</f>
+        <v>12.25</v>
+      </c>
+      <c r="G4">
+        <f>POWER(E4,2)</f>
+        <v>596756.25</v>
+      </c>
+      <c r="H4">
+        <f>D4*E4</f>
+        <v>2703.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="17">
+        <v>400</v>
+      </c>
+      <c r="D5">
+        <f>B5-$B$13</f>
+        <v>-2.5</v>
+      </c>
+      <c r="E5" s="17">
+        <f>C5-$C$13</f>
+        <v>-572.5</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:G11" si="0">POWER(D5,2)</f>
+        <v>6.25</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>327756.25</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H11" si="1">D5*E5</f>
+        <v>1431.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="17">
+        <v>725</v>
+      </c>
+      <c r="D6">
+        <f>B6-$B$13</f>
+        <v>-1.5</v>
+      </c>
+      <c r="E6" s="17">
+        <f>C6-$C$13</f>
+        <v>-247.5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>61256.25</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>371.25</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="17">
+        <v>915</v>
+      </c>
+      <c r="D7">
+        <f>B7-$B$13</f>
+        <v>-0.5</v>
+      </c>
+      <c r="E7" s="17">
+        <f>C7-$C$13</f>
+        <v>-57.5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>3306.25</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>28.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="17">
+        <v>990</v>
+      </c>
+      <c r="D8">
+        <f>B8-$B$13</f>
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="17">
+        <f>C8-$C$13</f>
+        <v>17.5</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>306.25</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="17">
+        <v>1300</v>
+      </c>
+      <c r="D9">
+        <f>B9-$B$13</f>
+        <v>1.5</v>
+      </c>
+      <c r="E9" s="17">
+        <f>C9-$C$13</f>
+        <v>327.5</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>107256.25</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>491.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="17">
+        <v>1600</v>
+      </c>
+      <c r="D10">
+        <f>B10-$B$13</f>
+        <v>2.5</v>
+      </c>
+      <c r="E10" s="17">
+        <f>C10-$C$13</f>
+        <v>627.5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>393756.25</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>1568.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="17">
+        <v>1650</v>
+      </c>
+      <c r="D11">
+        <f>B11-$B$13</f>
+        <v>3.5</v>
+      </c>
+      <c r="E11" s="17">
+        <f>C11-$C$13</f>
+        <v>677.5</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>12.25</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>459006.25</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>2371.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="18" t="str">
+        <f>D3</f>
+        <v>X-X'</v>
+      </c>
+      <c r="E12" s="18" t="str">
+        <f>E3</f>
+        <v>Y-Y'</v>
+      </c>
+      <c r="F12" s="18" t="str">
+        <f>F3</f>
+        <v>(X-X')2</v>
+      </c>
+      <c r="G12" s="18" t="str">
+        <f>G3</f>
+        <v>(Y-Y')2</v>
+      </c>
+      <c r="H12" s="18" t="str">
+        <f>H3</f>
+        <v>(X-X')*(Y-Y')</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="15">
+        <f>AVERAGE(B4:B11)</f>
+        <v>4.5</v>
+      </c>
+      <c r="C13" s="15">
+        <f>AVERAGE(C4:C11)</f>
+        <v>972.5</v>
+      </c>
+      <c r="D13" s="15">
+        <f>AVERAGE(D4:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="15">
+        <f>AVERAGE(E4:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="15">
+        <f>AVERAGE(F4:F11)</f>
+        <v>5.25</v>
+      </c>
+      <c r="G13" s="15">
+        <f>AVERAGE(G4:G11)</f>
+        <v>243675</v>
+      </c>
+      <c r="H13" s="15">
+        <f>AVERAGE(H4:H11)</f>
+        <v>1121.875</v>
+      </c>
+      <c r="M13" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="N13" s="32"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15">
+        <f>SUM(F4:F11)</f>
+        <v>42</v>
+      </c>
+      <c r="G15" s="15">
+        <f>SUM(G4:G11)</f>
+        <v>1949400</v>
+      </c>
+      <c r="H15" s="15">
+        <f>SUM(H4:H11)</f>
+        <v>8975</v>
+      </c>
+      <c r="M15" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="32"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15">
+        <f>F15/(n-1)</f>
+        <v>3.8181818181818183</v>
+      </c>
+      <c r="G17" s="15">
+        <f>G15/(n-1)</f>
+        <v>177218.18181818182</v>
+      </c>
+      <c r="H17" s="15"/>
+      <c r="M17" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" s="32"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15">
+        <f>SQRT(F17)</f>
+        <v>1.9540168418367889</v>
+      </c>
+      <c r="G19" s="15">
+        <f t="shared" ref="G19" si="2">SQRT(G17)</f>
+        <v>420.97289914931793</v>
+      </c>
+      <c r="H19" s="15"/>
+      <c r="M19" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="N19" s="32"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15">
+        <f>H15/(K6-1)</f>
+        <v>815.90909090909088</v>
+      </c>
+      <c r="M21" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="N21" s="32"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J22" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22">
+        <f>H21/(F19*G19)</f>
+        <v>0.99188045182977025</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" s="36">
+        <f>CORREL(B4:B11,C4:C11)</f>
+        <v>0.99188045182977036</v>
+      </c>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="N23" s="32"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="26">
+        <f>(H23*G19)/F19</f>
+        <v>213.69047619047618</v>
+      </c>
+      <c r="M25" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="N25" s="32"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="27">
+        <f>C13-(H25*B13)</f>
+        <v>10.892857142857224</v>
+      </c>
+      <c r="M27" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="N27" s="32"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I29" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="43"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="18" t="str">
+        <f>B3</f>
+        <v>Week</v>
+      </c>
+      <c r="C34" s="18" t="str">
+        <f>C3</f>
+        <v>Total Savings</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <f>($H$25*B35)+$H$27</f>
+        <v>224.5833333333334</v>
+      </c>
+      <c r="D35" s="30">
+        <f>C4-C35</f>
+        <v>-24.5833333333334</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:C37" si="3">($H$25*B36)+$H$27</f>
+        <v>438.27380952380958</v>
+      </c>
+      <c r="D36" s="30">
+        <f>C5-C36</f>
+        <v>-38.273809523809575</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="3"/>
+        <v>651.96428571428578</v>
+      </c>
+      <c r="D37" s="30">
+        <f>C6-C37</f>
+        <v>73.035714285714221</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="I29:M30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M19:N19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C1" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="34"/>
+      <c r="J1" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="43"/>
+    </row>
+    <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="E3">
+        <f>C3-$C$12</f>
+        <v>-3.5</v>
+      </c>
+      <c r="F3">
+        <f>D3-$D$12</f>
+        <v>-772.5</v>
+      </c>
+      <c r="G3">
+        <f>POWER(E3,2)</f>
+        <v>12.25</v>
+      </c>
+      <c r="H3">
+        <f>POWER(F3,2)</f>
+        <v>596756.25</v>
+      </c>
+      <c r="I3" s="44">
+        <f>E3*F3</f>
+        <v>2703.75</v>
+      </c>
+      <c r="J3" s="47">
+        <v>1</v>
+      </c>
+      <c r="K3" s="48">
+        <f>($I$24*J3)+$I$26</f>
+        <v>224.58333333333314</v>
+      </c>
+      <c r="L3" s="47">
+        <f>K3-D3</f>
+        <v>24.583333333333144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>400</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E10" si="0">C4-$C$12</f>
+        <v>-2.5</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F10" si="1">D4-$D$12</f>
+        <v>-572.5</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:H10" si="2">POWER(E4,2)</f>
+        <v>6.25</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>327756.25</v>
+      </c>
+      <c r="I4" s="44">
+        <f t="shared" ref="I4:I10" si="3">E4*F4</f>
+        <v>1431.25</v>
+      </c>
+      <c r="J4" s="16">
+        <v>2</v>
+      </c>
+      <c r="K4" s="48">
+        <f t="shared" ref="K4:K10" si="4">($I$24*J4)+$I$26</f>
+        <v>438.2738095238094</v>
+      </c>
+      <c r="L4" s="47">
+        <f>K4-D4</f>
+        <v>38.273809523809405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>725</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>-1.5</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>-247.5</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>61256.25</v>
+      </c>
+      <c r="I5" s="44">
+        <f t="shared" si="3"/>
+        <v>371.25</v>
+      </c>
+      <c r="J5" s="16">
+        <v>3</v>
+      </c>
+      <c r="K5" s="48">
+        <f t="shared" si="4"/>
+        <v>651.96428571428567</v>
+      </c>
+      <c r="L5" s="47">
+        <f>K5-D5</f>
+        <v>-73.035714285714334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>915</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>-57.5</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>3306.25</v>
+      </c>
+      <c r="I6" s="44">
+        <f t="shared" si="3"/>
+        <v>28.75</v>
+      </c>
+      <c r="J6" s="47">
+        <v>4</v>
+      </c>
+      <c r="K6" s="48">
+        <f>($I$24*J6)+$I$26</f>
+        <v>865.65476190476193</v>
+      </c>
+      <c r="L6" s="47">
+        <f>K6-D6</f>
+        <v>-49.345238095238074</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>990</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>17.5</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>306.25</v>
+      </c>
+      <c r="I7" s="44">
+        <f t="shared" si="3"/>
+        <v>8.75</v>
+      </c>
+      <c r="J7" s="16">
+        <v>5</v>
+      </c>
+      <c r="K7" s="48">
+        <f t="shared" si="4"/>
+        <v>1079.3452380952381</v>
+      </c>
+      <c r="L7" s="47">
+        <f>K7-D7</f>
+        <v>89.345238095238074</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>1300</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>327.5</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>107256.25</v>
+      </c>
+      <c r="I8" s="44">
+        <f t="shared" si="3"/>
+        <v>491.25</v>
+      </c>
+      <c r="J8" s="16">
+        <v>6</v>
+      </c>
+      <c r="K8" s="48">
+        <f t="shared" si="4"/>
+        <v>1293.0357142857144</v>
+      </c>
+      <c r="L8" s="47">
+        <f>K8-D8</f>
+        <v>-6.9642857142855519</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>1600</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>627.5</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>6.25</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>393756.25</v>
+      </c>
+      <c r="I9" s="44">
+        <f t="shared" si="3"/>
+        <v>1568.75</v>
+      </c>
+      <c r="J9" s="47">
+        <v>7</v>
+      </c>
+      <c r="K9" s="48">
+        <f>($I$24*J9)+$I$26</f>
+        <v>1506.7261904761908</v>
+      </c>
+      <c r="L9" s="47">
+        <f>K9-D9</f>
+        <v>-93.273809523809177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>1650</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>677.5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>12.25</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>459006.25</v>
+      </c>
+      <c r="I10" s="44">
+        <f t="shared" si="3"/>
+        <v>2371.25</v>
+      </c>
+      <c r="J10" s="16">
+        <v>8</v>
+      </c>
+      <c r="K10" s="48">
+        <f t="shared" si="4"/>
+        <v>1720.416666666667</v>
+      </c>
+      <c r="L10" s="47">
+        <f>K10-D10</f>
+        <v>70.41666666666697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="18" t="str">
+        <f>E2</f>
+        <v>X-X'</v>
+      </c>
+      <c r="F11" s="18" t="str">
+        <f>F2</f>
+        <v>Y-Y'</v>
+      </c>
+      <c r="G11" s="18" t="str">
+        <f>G2</f>
+        <v>(X-X')2</v>
+      </c>
+      <c r="H11" s="18" t="str">
+        <f>H2</f>
+        <v>(Y-Y')2</v>
+      </c>
+      <c r="I11" s="18" t="str">
+        <f>I2</f>
+        <v>(X-X')*(Y-Y')</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="15">
+        <f>AVERAGE(C3:C10)</f>
+        <v>4.5</v>
+      </c>
+      <c r="D12" s="15">
+        <f t="shared" ref="D12:I12" si="5">AVERAGE(D3:D10)</f>
+        <v>972.5</v>
+      </c>
+      <c r="E12" s="15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="15">
+        <f t="shared" si="5"/>
+        <v>5.25</v>
+      </c>
+      <c r="H12" s="15">
+        <f t="shared" si="5"/>
+        <v>243675</v>
+      </c>
+      <c r="I12" s="45">
+        <f t="shared" si="5"/>
+        <v>1121.875</v>
+      </c>
+      <c r="K12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I13" s="44"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15">
+        <f>SUM(G3:G10)</f>
+        <v>42</v>
+      </c>
+      <c r="H14" s="45">
+        <f>SUM(H3:H10)</f>
+        <v>1949400</v>
+      </c>
+      <c r="I14" s="45">
+        <f>SUM(I3:I10)</f>
+        <v>8975</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I15" s="44"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15">
+        <f>G14/(n-1)</f>
+        <v>6</v>
+      </c>
+      <c r="H16" s="45">
+        <f>H14/(n-1)</f>
+        <v>278485.71428571426</v>
+      </c>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I17" s="44"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15">
+        <f>SQRT(G16)</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="H18" s="45">
+        <f>SQRT(H16)</f>
+        <v>527.71745687035434</v>
+      </c>
+      <c r="I18" s="15"/>
+      <c r="K18" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I19" s="44"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="45">
+        <f>I14/(n-1)</f>
+        <v>1282.1428571428571</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K21" s="51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15">
+        <f>I20/(G18*H18)</f>
+        <v>0.99188045182977036</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22">
+        <f>CORREL(C3:C10,D3:D10)</f>
+        <v>0.99188045182977036</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K23" s="51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="27">
+        <f>(I22*H18)/G18</f>
+        <v>213.69047619047626</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24">
+        <f>SLOPE(D3:D10,C3:C10)</f>
+        <v>213.6904761904762</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J25" s="16"/>
+      <c r="K25" s="51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="46">
+        <f>D12-(I24*C12)</f>
+        <v>10.892857142856883</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" s="49">
+        <f>INTERCEPT(D3:D10,C3:C10)</f>
+        <v>10.89285714285711</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="K18:N19"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W31"/>
   <sheetViews>
@@ -5378,78 +7211,78 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
     </row>
@@ -6088,7 +7921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -6191,7 +8024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O23"/>
   <sheetViews>
@@ -6222,20 +8055,20 @@
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -6300,60 +8133,60 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="42">
         <f>MAX(B6:O6)</f>
         <v>100</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="42">
         <f>MIN(B6:O6)</f>
         <v>29</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
@@ -6436,53 +8269,53 @@
       </c>
     </row>
     <row r="19" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
     </row>
   </sheetData>
   <sortState ref="B13:O13">
@@ -6499,53 +8332,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="25">
-        <v>1</v>
-      </c>
-      <c r="C2" s="25"/>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="26">
-        <v>0.83024548881658111</v>
-      </c>
-      <c r="C3" s="26">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>